<commit_message>
Setting up output file information
</commit_message>
<xml_diff>
--- a/products.xlsx
+++ b/products.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\usgarretan2\Downloads\Testing\EasyInventory\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\usgarretan2\Downloads\Testing\EasyPartials\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{548B0AAB-A27F-43B8-B80B-8E635544BE2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3255B7FA-402D-4C77-9244-96CE8D361A76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5231EC94-5F99-4FCD-B062-71A2B22C17ED}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5231EC94-5F99-4FCD-B062-71A2B22C17ED}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -388,7 +388,7 @@
   <dimension ref="A1:B81"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:B81"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -486,7 +486,7 @@
         <v>11007819</v>
       </c>
       <c r="B12">
-        <v>140</v>
+        <v>100</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>